<commit_message>
Updated real value for north dakota 2024
</commit_message>
<xml_diff>
--- a/param/Variable_Dist.xlsx
+++ b/param/Variable_Dist.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jerry/Downloads/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/168116ed77ffbf42/Zhiwei_Song/Wisconsin/CS719_Final_Project/param/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A67AD50-608A-6B47-A8D8-DBF7B333CF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{8A67AD50-608A-6B47-A8D8-DBF7B333CF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F492FBF0-4F80-F64E-B0FB-148DE6628156}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17380" xr2:uid="{F566C3DC-534D-F345-8BF6-1AF6242EF834}"/>
+    <workbookView xWindow="11660" yWindow="1040" windowWidth="28040" windowHeight="17380" xr2:uid="{F566C3DC-534D-F345-8BF6-1AF6242EF834}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Type</t>
   </si>
@@ -84,6 +84,24 @@
   </si>
   <si>
     <t>RAINFALL</t>
+  </si>
+  <si>
+    <t>A=1500</t>
+  </si>
+  <si>
+    <t>B=30/20</t>
+  </si>
+  <si>
+    <t>C=8</t>
+  </si>
+  <si>
+    <t>alpha = 0.95</t>
+  </si>
+  <si>
+    <t>lambda = 0.5</t>
+  </si>
+  <si>
+    <t>North Dakota (2024)</t>
   </si>
 </sst>
 </file>
@@ -462,19 +480,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C90D34-C0E7-C148-9A75-B91E7DC9342C}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,9 +505,11 @@
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -497,8 +519,19 @@
       <c r="C2" s="1">
         <v>1.9612920911140801</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" s="1">
+        <v>17.8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -508,8 +541,11 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -519,8 +555,14 @@
       <c r="C5">
         <v>0.44203502736382499</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="1">
+        <v>4.21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -530,8 +572,14 @@
       <c r="C6">
         <v>1.3313311780175201</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="1">
+        <v>9.44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -541,8 +589,11 @@
       <c r="C7">
         <v>0.57817756698371703</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" s="1">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -552,8 +603,11 @@
       <c r="C8">
         <v>0.41587825435021603</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="1">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -563,8 +617,11 @@
       <c r="C9">
         <v>0.32035861848643898</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="1">
+        <v>5.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -574,8 +631,9 @@
       <c r="C10">
         <v>9.7818756963066501E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -585,8 +643,11 @@
       <c r="C11">
         <v>4.1545093404218596</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -597,7 +658,7 @@
         <v>5.3101145682885799E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -608,7 +669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -618,8 +679,11 @@
       <c r="C15">
         <v>16.452608709056801</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -629,8 +693,11 @@
       <c r="C16">
         <v>5.1063685726747101</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -640,8 +707,11 @@
       <c r="C17">
         <v>4.1427728234440604</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -651,8 +721,11 @@
       <c r="C18">
         <v>4.17622237594375</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -662,8 +735,11 @@
       <c r="C19">
         <v>7.0082166062415601</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -674,7 +750,7 @@
         <v>502.73850061438498</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -684,8 +760,11 @@
       <c r="C21">
         <v>9.5175276901794906E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -696,7 +775,7 @@
         <v>75.253460607026796</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -704,7 +783,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -713,7 +792,7 @@
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -721,7 +800,7 @@
         <v>21.653555000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -729,7 +808,7 @@
         <v>21.653555000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -737,7 +816,7 @@
         <v>39.370100000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -745,7 +824,7 @@
         <v>23.622060000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
@@ -753,7 +832,7 @@
         <v>22.637806999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -761,7 +840,7 @@
         <v>26.334499999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>